<commit_message>
Add the resulting Excel file
upd 2020-05-29
</commit_message>
<xml_diff>
--- a/tinkoff_data.xlsx
+++ b/tinkoff_data.xlsx
@@ -1394,7 +1394,7 @@
         <v>95</v>
       </c>
       <c r="AA7" s="4" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AB7" s="4" t="n">
         <v>75</v>
@@ -3401,7 +3401,7 @@
         <v>100</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S25" s="4" t="n">
         <v>100</v>
@@ -3701,7 +3701,7 @@
         <v>94</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F28" s="4" t="n">
         <v>95</v>
@@ -3945,7 +3945,7 @@
         <v>70</v>
       </c>
       <c r="K30" s="4" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L30" s="4" t="n">
         <v>81</v>
@@ -3990,7 +3990,7 @@
         <v>136</v>
       </c>
       <c r="Z30" s="4" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AA30" s="4" t="n">
         <v>112</v>
@@ -4469,7 +4469,7 @@
         <v>96</v>
       </c>
       <c r="AI34" s="4" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AJ34" s="4" t="n">
         <v>169</v>
@@ -6018,7 +6018,7 @@
         <v>40</v>
       </c>
       <c r="X48" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y48" s="4" t="n">
         <v>54</v>
@@ -8156,7 +8156,7 @@
         <v>70</v>
       </c>
       <c r="U67" s="4" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V67" s="4" t="n">
         <v>31</v>
@@ -11537,7 +11537,7 @@
         <v>33</v>
       </c>
       <c r="R97" s="4" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S97" s="4" t="n">
         <v>110</v>
@@ -12982,7 +12982,7 @@
         <v>11</v>
       </c>
       <c r="J110" s="4" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K110" s="4" t="n">
         <v>117</v>
@@ -13375,10 +13375,10 @@
         <v>129</v>
       </c>
       <c r="AB113" s="4" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC113" s="4" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD113" s="4" t="n">
         <v>135</v>
@@ -13396,7 +13396,7 @@
         <v>60</v>
       </c>
       <c r="AI113" s="4" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AJ113" s="4" t="n">
         <v>75</v>
@@ -13509,7 +13509,7 @@
         <v>59</v>
       </c>
       <c r="AI114" s="4" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AJ114" s="4" t="n">
         <v>71</v>
@@ -13544,7 +13544,7 @@
         <v>66</v>
       </c>
       <c r="I115" s="4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J115" s="4" t="n">
         <v>38</v>
@@ -13657,7 +13657,7 @@
         <v>85</v>
       </c>
       <c r="I116" s="4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J116" s="4" t="n">
         <v>93</v>
@@ -13678,7 +13678,7 @@
         <v>7</v>
       </c>
       <c r="P116" s="4" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q116" s="4" t="n">
         <v>45</v>
@@ -13687,13 +13687,13 @@
         <v>77</v>
       </c>
       <c r="S116" s="4" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="T116" s="4" t="n">
         <v>81</v>
       </c>
       <c r="U116" s="4" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="V116" s="4" t="n">
         <v>62</v>
@@ -13708,7 +13708,7 @@
         <v>32</v>
       </c>
       <c r="Z116" s="4" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA116" s="4" t="n">
         <v>131</v>
@@ -13735,13 +13735,352 @@
         <v>47</v>
       </c>
       <c r="AI116" s="4" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AJ116" s="4" t="n">
         <v>74</v>
       </c>
       <c r="AK116" s="4" t="n">
         <v>106</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>43977</v>
+      </c>
+      <c r="B117" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="C117" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D117" s="4" t="n">
+        <v>84</v>
+      </c>
+      <c r="E117" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>139</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>89</v>
+      </c>
+      <c r="I117" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J117" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="K117" s="4" t="n">
+        <v>118</v>
+      </c>
+      <c r="L117" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="M117" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="N117" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="O117" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="P117" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q117" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="R117" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="S117" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="T117" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="U117" s="4" t="n">
+        <v>113</v>
+      </c>
+      <c r="V117" s="4" t="n">
+        <v>71</v>
+      </c>
+      <c r="W117" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="X117" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y117" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Z117" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="AA117" s="4" t="n">
+        <v>144</v>
+      </c>
+      <c r="AB117" s="4" t="n">
+        <v>76</v>
+      </c>
+      <c r="AC117" s="4" t="n">
+        <v>58</v>
+      </c>
+      <c r="AD117" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="AE117" s="4" t="n">
+        <v>97</v>
+      </c>
+      <c r="AF117" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AG117" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH117" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AI117" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="AJ117" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="AK117" s="4" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>43978</v>
+      </c>
+      <c r="B118" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="C118" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D118" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="E118" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F118" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="G118" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="H118" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="I118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="J118" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="K118" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="L118" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="M118" s="4" t="n">
+        <v>119</v>
+      </c>
+      <c r="N118" s="4" t="n">
+        <v>91</v>
+      </c>
+      <c r="O118" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="P118" s="4" t="n">
+        <v>78</v>
+      </c>
+      <c r="Q118" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="R118" s="4" t="n">
+        <v>82</v>
+      </c>
+      <c r="S118" s="4" t="n">
+        <v>107</v>
+      </c>
+      <c r="T118" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="U118" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="V118" s="4" t="n">
+        <v>72</v>
+      </c>
+      <c r="W118" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="X118" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y118" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z118" s="4" t="n">
+        <v>113</v>
+      </c>
+      <c r="AA118" s="4" t="n">
+        <v>133</v>
+      </c>
+      <c r="AB118" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="AC118" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="AD118" s="4" t="n">
+        <v>109</v>
+      </c>
+      <c r="AE118" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="AF118" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="AG118" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH118" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="AI118" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="AJ118" s="4" t="n">
+        <v>67</v>
+      </c>
+      <c r="AK118" s="4" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>43979</v>
+      </c>
+      <c r="B119" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="C119" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D119" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="E119" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F119" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G119" s="4" t="n">
+        <v>154</v>
+      </c>
+      <c r="H119" s="4" t="n">
+        <v>87</v>
+      </c>
+      <c r="I119" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J119" s="4" t="n">
+        <v>92</v>
+      </c>
+      <c r="K119" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="L119" s="4" t="n">
+        <v>44</v>
+      </c>
+      <c r="M119" s="4" t="n">
+        <v>123</v>
+      </c>
+      <c r="N119" s="4" t="n">
+        <v>69</v>
+      </c>
+      <c r="O119" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="P119" s="4" t="n">
+        <v>74</v>
+      </c>
+      <c r="Q119" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="R119" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="S119" s="4" t="n">
+        <v>123</v>
+      </c>
+      <c r="T119" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="U119" s="4" t="n">
+        <v>119</v>
+      </c>
+      <c r="V119" s="4" t="n">
+        <v>74</v>
+      </c>
+      <c r="W119" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="X119" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y119" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z119" s="4" t="n">
+        <v>113</v>
+      </c>
+      <c r="AA119" s="4" t="n">
+        <v>126</v>
+      </c>
+      <c r="AB119" s="4" t="n">
+        <v>83</v>
+      </c>
+      <c r="AC119" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="AD119" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="AE119" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="AF119" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AG119" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH119" s="4" t="n">
+        <v>54</v>
+      </c>
+      <c r="AI119" s="4" t="n">
+        <v>82</v>
+      </c>
+      <c r="AJ119" s="4" t="n">
+        <v>69</v>
+      </c>
+      <c r="AK119" s="4" t="n">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -20337,6 +20676,138 @@
       <c r="AO116" s="4"/>
       <c r="AP116" s="4"/>
     </row>
+    <row r="117">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="4"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+      <c r="U117" s="4"/>
+      <c r="V117" s="4"/>
+      <c r="W117" s="4"/>
+      <c r="X117" s="4"/>
+      <c r="Y117" s="4"/>
+      <c r="Z117" s="4"/>
+      <c r="AA117" s="4"/>
+      <c r="AB117" s="4"/>
+      <c r="AC117" s="4"/>
+      <c r="AD117" s="4"/>
+      <c r="AE117" s="4"/>
+      <c r="AF117" s="4"/>
+      <c r="AG117" s="4"/>
+      <c r="AH117" s="4"/>
+      <c r="AI117" s="4"/>
+      <c r="AJ117" s="4"/>
+      <c r="AK117" s="4"/>
+      <c r="AL117" s="4"/>
+      <c r="AM117" s="4"/>
+      <c r="AN117" s="4"/>
+      <c r="AO117" s="4"/>
+      <c r="AP117" s="4"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
+      <c r="X118" s="4"/>
+      <c r="Y118" s="4"/>
+      <c r="Z118" s="4"/>
+      <c r="AA118" s="4"/>
+      <c r="AB118" s="4"/>
+      <c r="AC118" s="4"/>
+      <c r="AD118" s="4"/>
+      <c r="AE118" s="4"/>
+      <c r="AF118" s="4"/>
+      <c r="AG118" s="4"/>
+      <c r="AH118" s="4"/>
+      <c r="AI118" s="4"/>
+      <c r="AJ118" s="4"/>
+      <c r="AK118" s="4"/>
+      <c r="AL118" s="4"/>
+      <c r="AM118" s="4"/>
+      <c r="AN118" s="4"/>
+      <c r="AO118" s="4"/>
+      <c r="AP118" s="4"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="4"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+      <c r="U119" s="4"/>
+      <c r="V119" s="4"/>
+      <c r="W119" s="4"/>
+      <c r="X119" s="4"/>
+      <c r="Y119" s="4"/>
+      <c r="Z119" s="4"/>
+      <c r="AA119" s="4"/>
+      <c r="AB119" s="4"/>
+      <c r="AC119" s="4"/>
+      <c r="AD119" s="4"/>
+      <c r="AE119" s="4"/>
+      <c r="AF119" s="4"/>
+      <c r="AG119" s="4"/>
+      <c r="AH119" s="4"/>
+      <c r="AI119" s="4"/>
+      <c r="AJ119" s="4"/>
+      <c r="AK119" s="4"/>
+      <c r="AL119" s="4"/>
+      <c r="AM119" s="4"/>
+      <c r="AN119" s="4"/>
+      <c r="AO119" s="4"/>
+      <c r="AP119" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>